<commit_message>
Update problem 33 and 69
</commit_message>
<xml_diff>
--- a/Python_LeetCode/花花酱 LeetCode 题目分类 _ youtube.com_user_xxfflower .xlsx
+++ b/Python_LeetCode/花花酱 LeetCode 题目分类 _ youtube.com_user_xxfflower .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ba6ca2776cfd04a2/Projects/DevOps/Notes/DevOps-learning-notes/Python_LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="134" documentId="11_06CFFED9B2426DA59DEC10EDCE3DB48FCB33D6CA" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CBECB0F7-73D8-43DF-8A20-E33006F25E9C}"/>
+  <xr:revisionPtr revIDLastSave="157" documentId="11_06CFFED9B2426DA59DEC10EDCE3DB48FCB33D6CA" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ED19E241-83E6-4E9C-AD09-11D039E58056}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="884" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -274,7 +274,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="91">
   <si>
     <t>Id</t>
   </si>
@@ -544,12 +544,21 @@
   <si>
     <t>*</t>
   </si>
+  <si>
+    <t>1008.Construct Binary Search Tree from Preorder Traversal</t>
+  </si>
+  <si>
+    <t>33.Search in Rotated Sorted Array.</t>
+  </si>
+  <si>
+    <t>69. Sqrt(x)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="37" x14ac:knownFonts="1">
+  <fonts count="38" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -765,6 +774,12 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1133,7 +1148,7 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1152,16 +1167,16 @@
     <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1169,7 +1184,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1485,10 +1500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB87F8D1-CF69-4679-BA35-9F173745AC62}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1543,12 +1558,14 @@
       <c r="D3" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="E3" s="70"/>
+      <c r="E3" s="67" t="s">
+        <v>87</v>
+      </c>
       <c r="F3" s="70"/>
       <c r="G3" s="70"/>
     </row>
     <row r="4" spans="1:7" s="60" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="91" t="s">
         <v>79</v>
       </c>
       <c r="B4" s="67" t="s">
@@ -1557,7 +1574,9 @@
       <c r="C4" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="69"/>
+      <c r="D4" s="67" t="s">
+        <v>87</v>
+      </c>
       <c r="E4" s="70"/>
       <c r="F4" s="70"/>
       <c r="G4" s="70"/>
@@ -1584,7 +1603,7 @@
     </row>
     <row r="7" spans="1:7" s="60" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="65" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B7" s="67" t="s">
         <v>87</v>
@@ -1592,14 +1611,18 @@
       <c r="C7" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="69"/>
-      <c r="E7" s="70"/>
+      <c r="D7" s="67" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" s="67" t="s">
+        <v>87</v>
+      </c>
       <c r="F7" s="70"/>
       <c r="G7" s="70"/>
     </row>
     <row r="8" spans="1:7" s="60" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="65" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B8" s="67" t="s">
         <v>87</v>
@@ -1610,13 +1633,15 @@
       <c r="D8" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="E8" s="70"/>
+      <c r="E8" s="67" t="s">
+        <v>87</v>
+      </c>
       <c r="F8" s="70"/>
       <c r="G8" s="70"/>
     </row>
     <row r="9" spans="1:7" s="60" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="65" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B9" s="67" t="s">
         <v>87</v>
@@ -1633,7 +1658,7 @@
     </row>
     <row r="10" spans="1:7" s="60" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="65" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B10" s="67" t="s">
         <v>87</v>
@@ -1641,14 +1666,16 @@
       <c r="C10" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="D10" s="69"/>
+      <c r="D10" s="67" t="s">
+        <v>87</v>
+      </c>
       <c r="E10" s="70"/>
       <c r="F10" s="70"/>
       <c r="G10" s="70"/>
     </row>
     <row r="11" spans="1:7" s="60" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="65" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B11" s="67" t="s">
         <v>87</v>
@@ -1656,16 +1683,14 @@
       <c r="C11" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="D11" s="69"/>
+      <c r="D11" s="67" t="s">
+        <v>87</v>
+      </c>
       <c r="E11" s="70"/>
       <c r="F11" s="70"/>
       <c r="G11" s="70"/>
     </row>
     <row r="12" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="75"/>
-      <c r="B12" s="69"/>
-      <c r="C12" s="69"/>
-      <c r="D12" s="69"/>
       <c r="E12" s="70"/>
       <c r="F12" s="70"/>
       <c r="G12" s="70"/>
@@ -1691,10 +1716,41 @@
       <c r="C14" s="67" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D14" s="67" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="73">
+        <v>43941</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="65" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="67" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="65" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D19" s="69" t="s">
         <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="73">
+        <v>43942</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="65" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -22604,7 +22660,7 @@
   <dimension ref="A1:I1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -27901,7 +27957,7 @@
   <dimension ref="A1:I1013"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -27956,7 +28012,7 @@
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
-      <c r="I2" s="84" t="s">
+      <c r="I2" s="85" t="s">
         <v>8</v>
       </c>
     </row>
@@ -27979,7 +28035,7 @@
       <c r="F3" s="15"/>
       <c r="G3" s="16"/>
       <c r="H3" s="15"/>
-      <c r="I3" s="85"/>
+      <c r="I3" s="87"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
@@ -28033,7 +28089,7 @@
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/dynamic-programming/leetcode-931-minimum-falling-path-sum/","931")</f>
         <v>931</v>
       </c>
-      <c r="I5" s="84" t="s">
+      <c r="I5" s="85" t="s">
         <v>14</v>
       </c>
     </row>
@@ -28049,7 +28105,7 @@
       <c r="F6" s="16"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
-      <c r="I6" s="85"/>
+      <c r="I6" s="87"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
@@ -28155,7 +28211,7 @@
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
-      <c r="I10" s="84" t="s">
+      <c r="I10" s="85" t="s">
         <v>20</v>
       </c>
     </row>
@@ -28181,7 +28237,7 @@
       <c r="F11" s="15"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
-      <c r="I11" s="85"/>
+      <c r="I11" s="87"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
@@ -28248,7 +28304,7 @@
       <c r="A15" s="79">
         <v>72</v>
       </c>
-      <c r="B15" s="87" t="str">
+      <c r="B15" s="84" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/dynamic-programming/leetcode-72-edit-distance/","Edit Distance")</f>
         <v>Edit Distance</v>
       </c>
@@ -28275,7 +28331,7 @@
         <f>HYPERLINK("https://leetcode.com/problems/delete-operation-for-two-strings/","583")</f>
         <v>583</v>
       </c>
-      <c r="I15" s="84" t="s">
+      <c r="I15" s="85" t="s">
         <v>25</v>
       </c>
     </row>
@@ -28382,7 +28438,7 @@
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/leetcode/leetcode-weekly-contest-137/","1049")</f>
         <v>1049</v>
       </c>
-      <c r="I19" s="84" t="s">
+      <c r="I19" s="85" t="s">
         <v>28</v>
       </c>
     </row>
@@ -34485,6 +34541,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="I5:I7"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C15:C16"/>
@@ -34493,13 +34556,6 @@
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="I19:I20"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="I5:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -34513,7 +34569,7 @@
   <dimension ref="A1:K999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -34583,7 +34639,7 @@
       <c r="A3" s="5">
         <v>33</v>
       </c>
-      <c r="B3" s="91" t="str">
+      <c r="B3" s="75" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/search-in-rotated-sorted-array","Search in Rotated Sorted Array")</f>
         <v>Search in Rotated Sorted Array</v>
       </c>
@@ -38752,7 +38808,7 @@
   <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="E14" sqref="E14:J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update problem Leftmost Column with at Least a One
</commit_message>
<xml_diff>
--- a/Python_LeetCode/花花酱 LeetCode 题目分类 _ youtube.com_user_xxfflower .xlsx
+++ b/Python_LeetCode/花花酱 LeetCode 题目分类 _ youtube.com_user_xxfflower .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ba6ca2776cfd04a2/Projects/DevOps/Notes/DevOps-learning-notes/Python_LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="157" documentId="11_06CFFED9B2426DA59DEC10EDCE3DB48FCB33D6CA" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ED19E241-83E6-4E9C-AD09-11D039E58056}"/>
+  <xr:revisionPtr revIDLastSave="161" documentId="11_06CFFED9B2426DA59DEC10EDCE3DB48FCB33D6CA" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DF6AFA82-7DE4-4DCF-B238-7F6367207A3B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="884" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="884" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily" sheetId="15" r:id="rId1"/>
@@ -274,7 +274,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="92">
   <si>
     <t>Id</t>
   </si>
@@ -552,6 +552,9 @@
   </si>
   <si>
     <t>69. Sqrt(x)</t>
+  </si>
+  <si>
+    <t>Leftmost Column with at Least a One</t>
   </si>
 </sst>
 </file>
@@ -1149,6 +1152,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1167,16 +1171,16 @@
     <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1184,7 +1188,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1500,10 +1503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB87F8D1-CF69-4679-BA35-9F173745AC62}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1565,7 +1568,7 @@
       <c r="G3" s="70"/>
     </row>
     <row r="4" spans="1:7" s="60" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="91" t="s">
+      <c r="A4" s="76" t="s">
         <v>79</v>
       </c>
       <c r="B4" s="67" t="s">
@@ -1748,9 +1751,22 @@
         <v>43942</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="65" t="s">
         <v>90</v>
+      </c>
+      <c r="B21" s="67" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="73">
+        <v>43943</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="65" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1830,15 +1846,15 @@
       <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="76" t="s">
+      <c r="D3" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="79"/>
       <c r="K3" s="5" t="s">
         <v>4</v>
       </c>
@@ -6068,15 +6084,15 @@
       <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="90" t="s">
+      <c r="D1" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
       <c r="K1" s="53" t="s">
         <v>4</v>
       </c>
@@ -10251,15 +10267,15 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="79"/>
       <c r="K1" s="5" t="s">
         <v>4</v>
       </c>
@@ -14423,13 +14439,13 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="79"/>
       <c r="I1" s="5" t="s">
         <v>4</v>
       </c>
@@ -18537,14 +18553,14 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="79"/>
       <c r="J1" s="5" t="s">
         <v>4</v>
       </c>
@@ -22660,7 +22676,7 @@
   <dimension ref="A1:I1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -22682,26 +22698,26 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="79"/>
       <c r="I1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="79">
+      <c r="A2" s="80">
         <v>94</v>
       </c>
-      <c r="B2" s="81" t="str">
+      <c r="B2" s="82" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/tree/leetcode-94-binary-tree-inorder-traversal/","Binary Tree Inorder Traversal")</f>
         <v>Binary Tree Inorder Traversal</v>
       </c>
-      <c r="C2" s="82" t="s">
+      <c r="C2" s="83" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="10" t="str">
@@ -22729,9 +22745,9 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="80"/>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
+      <c r="A3" s="81"/>
+      <c r="B3" s="81"/>
+      <c r="C3" s="81"/>
       <c r="D3" s="10" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/tree/leetcode-987-vertical-order-traversal-of-a-binary-tree/","987")</f>
         <v>987</v>
@@ -22746,14 +22762,14 @@
       <c r="I3" s="18"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="79">
+      <c r="A4" s="80">
         <v>100</v>
       </c>
-      <c r="B4" s="83" t="str">
+      <c r="B4" s="84" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/tree/leetcode-100-same-tree/","Same Tree")</f>
         <v>Same Tree</v>
       </c>
-      <c r="C4" s="82" t="s">
+      <c r="C4" s="83" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="9" t="str">
@@ -22779,9 +22795,9 @@
       <c r="I4" s="18"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="80"/>
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
+      <c r="A5" s="81"/>
+      <c r="B5" s="81"/>
+      <c r="C5" s="81"/>
       <c r="D5" s="29" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/univalued-binary-tree/","965")</f>
         <v>965</v>
@@ -27957,7 +27973,7 @@
   <dimension ref="A1:I1013"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -27979,13 +27995,13 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="79"/>
       <c r="I1" s="6" t="s">
         <v>4</v>
       </c>
@@ -28035,7 +28051,7 @@
       <c r="F3" s="15"/>
       <c r="G3" s="16"/>
       <c r="H3" s="15"/>
-      <c r="I3" s="87"/>
+      <c r="I3" s="86"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
@@ -28056,17 +28072,17 @@
       <c r="F4" s="15"/>
       <c r="G4" s="16"/>
       <c r="H4" s="15"/>
-      <c r="I4" s="80"/>
+      <c r="I4" s="81"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="79">
+      <c r="A5" s="80">
         <v>62</v>
       </c>
-      <c r="B5" s="86" t="str">
+      <c r="B5" s="87" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/dynamic-programming/leetcode-62-unique-paths/","Unique Paths")</f>
         <v>Unique Paths</v>
       </c>
-      <c r="C5" s="82" t="s">
+      <c r="C5" s="83" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="13" t="str">
@@ -28094,9 +28110,9 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="80"/>
-      <c r="B6" s="80"/>
-      <c r="C6" s="80"/>
+      <c r="A6" s="81"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="81"/>
       <c r="D6" s="14" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/searching/leetcode-1210-minimum-moves-to-reach-target-with-rotations/","1210")</f>
         <v>1210</v>
@@ -28105,7 +28121,7 @@
       <c r="F6" s="16"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
-      <c r="I6" s="87"/>
+      <c r="I6" s="86"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
@@ -28132,7 +28148,7 @@
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
-      <c r="I7" s="80"/>
+      <c r="I7" s="81"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
@@ -28237,7 +28253,7 @@
       <c r="F11" s="15"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
-      <c r="I11" s="87"/>
+      <c r="I11" s="86"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
@@ -28255,7 +28271,7 @@
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
-      <c r="I12" s="80"/>
+      <c r="I12" s="81"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
@@ -28301,14 +28317,14 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="79">
+      <c r="A15" s="80">
         <v>72</v>
       </c>
-      <c r="B15" s="84" t="str">
+      <c r="B15" s="88" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/dynamic-programming/leetcode-72-edit-distance/","Edit Distance")</f>
         <v>Edit Distance</v>
       </c>
-      <c r="C15" s="82" t="s">
+      <c r="C15" s="83" t="s">
         <v>7</v>
       </c>
       <c r="D15" s="14" t="str">
@@ -28336,9 +28352,9 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="80"/>
-      <c r="B16" s="80"/>
-      <c r="C16" s="80"/>
+      <c r="A16" s="81"/>
+      <c r="B16" s="81"/>
+      <c r="C16" s="81"/>
       <c r="D16" s="13" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/dynamic-programming/leetcode-712-minimum-ascii-delete-sum-for-two-strings/","712")</f>
         <v>712</v>
@@ -28359,7 +28375,7 @@
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/dynamic-programming/leetcode-718-maximum-length-of-repeated-subarray/","718")</f>
         <v>718</v>
       </c>
-      <c r="I16" s="80"/>
+      <c r="I16" s="81"/>
     </row>
     <row r="17" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
@@ -28408,14 +28424,14 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A19" s="79">
+      <c r="A19" s="80">
         <v>322</v>
       </c>
-      <c r="B19" s="86" t="str">
+      <c r="B19" s="87" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/dynamic-programming/leetcode-322-coin-change/","Coin Change")</f>
         <v>Coin Change</v>
       </c>
-      <c r="C19" s="82" t="s">
+      <c r="C19" s="83" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="10" t="str">
@@ -28443,9 +28459,9 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A20" s="80"/>
-      <c r="B20" s="80"/>
-      <c r="C20" s="80"/>
+      <c r="A20" s="81"/>
+      <c r="B20" s="81"/>
+      <c r="C20" s="81"/>
       <c r="D20" s="10" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/dynamic-programming/leetcode-1220-count-vowels-permutation/","1220")</f>
         <v>1220</v>
@@ -28463,7 +28479,7 @@
         <v>1269</v>
       </c>
       <c r="H20" s="15"/>
-      <c r="I20" s="80"/>
+      <c r="I20" s="81"/>
     </row>
     <row r="21" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
@@ -34541,13 +34557,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="I5:I7"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C15:C16"/>
@@ -34556,6 +34565,13 @@
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="I19:I20"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="I5:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -34568,8 +34584,8 @@
   </sheetPr>
   <dimension ref="A1:K999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -34591,15 +34607,15 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="79"/>
       <c r="K1" s="5" t="s">
         <v>4</v>
       </c>
@@ -38830,15 +38846,15 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="79"/>
       <c r="K1" s="5" t="s">
         <v>4</v>
       </c>
@@ -43120,13 +43136,13 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="79"/>
       <c r="I1" s="5" t="s">
         <v>4</v>
       </c>
@@ -48278,13 +48294,13 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="79"/>
       <c r="I1" s="33" t="s">
         <v>4</v>
       </c>
@@ -53690,15 +53706,15 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="79"/>
       <c r="K1" s="5" t="s">
         <v>4</v>
       </c>
@@ -57897,18 +57913,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="89" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
       <c r="K1" s="53"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -57958,15 +57974,15 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="76" t="s">
+      <c r="D4" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="77"/>
-      <c r="J4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="78"/>
+      <c r="J4" s="79"/>
       <c r="K4" s="5" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Update problem 146 and 201
</commit_message>
<xml_diff>
--- a/Python_LeetCode/花花酱 LeetCode 题目分类 _ youtube.com_user_xxfflower .xlsx
+++ b/Python_LeetCode/花花酱 LeetCode 题目分类 _ youtube.com_user_xxfflower .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ba6ca2776cfd04a2/Projects/DevOps/Notes/DevOps-learning-notes/Python_LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="161" documentId="11_06CFFED9B2426DA59DEC10EDCE3DB48FCB33D6CA" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DF6AFA82-7DE4-4DCF-B238-7F6367207A3B}"/>
+  <xr:revisionPtr revIDLastSave="180" documentId="11_06CFFED9B2426DA59DEC10EDCE3DB48FCB33D6CA" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1A3A03A1-5E02-44FD-B244-023DE9134081}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="884" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -274,7 +274,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="93">
   <si>
     <t>Id</t>
   </si>
@@ -555,6 +555,9 @@
   </si>
   <si>
     <t>Leftmost Column with at Least a One</t>
+  </si>
+  <si>
+    <t>560.Subarray Sum Equals K</t>
   </si>
 </sst>
 </file>
@@ -1171,16 +1174,16 @@
     <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1503,15 +1506,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB87F8D1-CF69-4679-BA35-9F173745AC62}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" style="65" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.109375" style="65" customWidth="1"/>
     <col min="2" max="4" width="4.77734375" style="69" customWidth="1"/>
     <col min="5" max="7" width="4.77734375" style="70" customWidth="1"/>
   </cols>
@@ -1564,7 +1568,9 @@
       <c r="E3" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="F3" s="70"/>
+      <c r="F3" s="67" t="s">
+        <v>87</v>
+      </c>
       <c r="G3" s="70"/>
     </row>
     <row r="4" spans="1:7" s="60" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -1620,7 +1626,9 @@
       <c r="E7" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="F7" s="70"/>
+      <c r="F7" s="67" t="s">
+        <v>87</v>
+      </c>
       <c r="G7" s="70"/>
     </row>
     <row r="8" spans="1:7" s="60" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -1639,11 +1647,13 @@
       <c r="E8" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="F8" s="70"/>
+      <c r="F8" s="67" t="s">
+        <v>87</v>
+      </c>
       <c r="G8" s="70"/>
     </row>
     <row r="9" spans="1:7" s="60" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="65" t="s">
+      <c r="A9" s="76" t="s">
         <v>83</v>
       </c>
       <c r="B9" s="67" t="s">
@@ -1655,7 +1665,9 @@
       <c r="D9" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="E9" s="70"/>
+      <c r="E9" s="67" t="s">
+        <v>87</v>
+      </c>
       <c r="F9" s="70"/>
       <c r="G9" s="70"/>
     </row>
@@ -1672,7 +1684,9 @@
       <c r="D10" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="E10" s="70"/>
+      <c r="E10" s="67" t="s">
+        <v>87</v>
+      </c>
       <c r="F10" s="70"/>
       <c r="G10" s="70"/>
     </row>
@@ -1689,7 +1703,9 @@
       <c r="D11" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="70"/>
+      <c r="E11" s="67" t="s">
+        <v>87</v>
+      </c>
       <c r="F11" s="70"/>
       <c r="G11" s="70"/>
     </row>
@@ -1722,6 +1738,9 @@
       <c r="D14" s="67" t="s">
         <v>87</v>
       </c>
+      <c r="E14" s="67" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="73">
@@ -1735,10 +1754,16 @@
       <c r="B17" s="67" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="67" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="65" t="s">
         <v>89</v>
+      </c>
+      <c r="B18" s="67" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1764,9 +1789,22 @@
         <v>43943</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="65" t="s">
         <v>91</v>
+      </c>
+      <c r="B24" s="67" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="73">
+        <v>43945</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="65" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -22676,7 +22714,7 @@
   <dimension ref="A1:I1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -27973,7 +28011,7 @@
   <dimension ref="A1:I1013"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -28028,7 +28066,7 @@
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
-      <c r="I2" s="85" t="s">
+      <c r="I2" s="86" t="s">
         <v>8</v>
       </c>
     </row>
@@ -28051,7 +28089,7 @@
       <c r="F3" s="15"/>
       <c r="G3" s="16"/>
       <c r="H3" s="15"/>
-      <c r="I3" s="86"/>
+      <c r="I3" s="88"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
@@ -28105,7 +28143,7 @@
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/dynamic-programming/leetcode-931-minimum-falling-path-sum/","931")</f>
         <v>931</v>
       </c>
-      <c r="I5" s="85" t="s">
+      <c r="I5" s="86" t="s">
         <v>14</v>
       </c>
     </row>
@@ -28121,7 +28159,7 @@
       <c r="F6" s="16"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
-      <c r="I6" s="86"/>
+      <c r="I6" s="88"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
@@ -28227,7 +28265,7 @@
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
-      <c r="I10" s="85" t="s">
+      <c r="I10" s="86" t="s">
         <v>20</v>
       </c>
     </row>
@@ -28253,7 +28291,7 @@
       <c r="F11" s="15"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
-      <c r="I11" s="86"/>
+      <c r="I11" s="88"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
@@ -28320,7 +28358,7 @@
       <c r="A15" s="80">
         <v>72</v>
       </c>
-      <c r="B15" s="88" t="str">
+      <c r="B15" s="85" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/dynamic-programming/leetcode-72-edit-distance/","Edit Distance")</f>
         <v>Edit Distance</v>
       </c>
@@ -28347,7 +28385,7 @@
         <f>HYPERLINK("https://leetcode.com/problems/delete-operation-for-two-strings/","583")</f>
         <v>583</v>
       </c>
-      <c r="I15" s="85" t="s">
+      <c r="I15" s="86" t="s">
         <v>25</v>
       </c>
     </row>
@@ -28454,7 +28492,7 @@
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/leetcode/leetcode-weekly-contest-137/","1049")</f>
         <v>1049</v>
       </c>
-      <c r="I19" s="85" t="s">
+      <c r="I19" s="86" t="s">
         <v>28</v>
       </c>
     </row>
@@ -34557,6 +34595,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="I5:I7"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C15:C16"/>
@@ -34565,13 +34610,6 @@
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="I19:I20"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="I5:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -34585,7 +34623,7 @@
   <dimension ref="A1:K999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update Install Jenkins instructions on Centos/Ubuntu and Update problem 124
</commit_message>
<xml_diff>
--- a/Python_LeetCode/花花酱 LeetCode 题目分类 _ youtube.com_user_xxfflower .xlsx
+++ b/Python_LeetCode/花花酱 LeetCode 题目分类 _ youtube.com_user_xxfflower .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ba6ca2776cfd04a2/Projects/DevOps/Notes/DevOps-learning-notes/Python_LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="185" documentId="11_06CFFED9B2426DA59DEC10EDCE3DB48FCB33D6CA" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DE17292E-BFB4-49B7-8971-A678E160B239}"/>
+  <xr:revisionPtr revIDLastSave="195" documentId="11_06CFFED9B2426DA59DEC10EDCE3DB48FCB33D6CA" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DC9330B2-0D6A-4F7D-ABD9-1A6259DB60CA}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="884" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="884" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily" sheetId="15" r:id="rId1"/>
@@ -274,7 +274,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="98">
   <si>
     <t>Id</t>
   </si>
@@ -564,6 +564,15 @@
   </si>
   <si>
     <t>201.Bitwise AND of Numbers Range</t>
+  </si>
+  <si>
+    <t>55.Jump Game</t>
+  </si>
+  <si>
+    <t>221.Maximal Square</t>
+  </si>
+  <si>
+    <t>1133.First Unique Number</t>
   </si>
 </sst>
 </file>
@@ -974,7 +983,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1162,6 +1171,7 @@
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1180,16 +1190,16 @@
     <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1512,11 +1522,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB87F8D1-CF69-4679-BA35-9F173745AC62}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1829,6 +1839,40 @@
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="65" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="73">
+        <v>43949</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="65" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="77" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="65"/>
+      <c r="B35" s="69"/>
+      <c r="C35" s="69"/>
+      <c r="D35" s="69"/>
+      <c r="E35" s="70"/>
+      <c r="F35" s="70"/>
+      <c r="G35" s="70"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="73">
+        <v>43947</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="65" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="65" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1908,15 +1952,15 @@
       <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="77" t="s">
+      <c r="D3" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="80"/>
       <c r="K3" s="5" t="s">
         <v>4</v>
       </c>
@@ -6146,15 +6190,15 @@
       <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="91" t="s">
+      <c r="D1" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="90"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
       <c r="K1" s="53" t="s">
         <v>4</v>
       </c>
@@ -10329,15 +10373,15 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="D1" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="80"/>
       <c r="K1" s="5" t="s">
         <v>4</v>
       </c>
@@ -14501,13 +14545,13 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="D1" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="80"/>
       <c r="I1" s="5" t="s">
         <v>4</v>
       </c>
@@ -18615,14 +18659,14 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="D1" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="80"/>
       <c r="J1" s="5" t="s">
         <v>4</v>
       </c>
@@ -22737,8 +22781,8 @@
   </sheetPr>
   <dimension ref="A1:I1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -22760,26 +22804,26 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="D1" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="80"/>
       <c r="I1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="80">
+      <c r="A2" s="81">
         <v>94</v>
       </c>
-      <c r="B2" s="82" t="str">
+      <c r="B2" s="83" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/tree/leetcode-94-binary-tree-inorder-traversal/","Binary Tree Inorder Traversal")</f>
         <v>Binary Tree Inorder Traversal</v>
       </c>
-      <c r="C2" s="83" t="s">
+      <c r="C2" s="84" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="10" t="str">
@@ -22807,9 +22851,9 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="81"/>
-      <c r="B3" s="81"/>
-      <c r="C3" s="81"/>
+      <c r="A3" s="82"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
       <c r="D3" s="10" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/tree/leetcode-987-vertical-order-traversal-of-a-binary-tree/","987")</f>
         <v>987</v>
@@ -22824,14 +22868,14 @@
       <c r="I3" s="18"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="80">
+      <c r="A4" s="81">
         <v>100</v>
       </c>
-      <c r="B4" s="84" t="str">
+      <c r="B4" s="85" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/tree/leetcode-100-same-tree/","Same Tree")</f>
         <v>Same Tree</v>
       </c>
-      <c r="C4" s="83" t="s">
+      <c r="C4" s="84" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="9" t="str">
@@ -22857,9 +22901,9 @@
       <c r="I4" s="18"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="81"/>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
+      <c r="A5" s="82"/>
+      <c r="B5" s="82"/>
+      <c r="C5" s="82"/>
       <c r="D5" s="29" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/univalued-binary-tree/","965")</f>
         <v>965</v>
@@ -28035,7 +28079,7 @@
   <dimension ref="A1:I1013"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -28057,13 +28101,13 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="D1" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="80"/>
       <c r="I1" s="6" t="s">
         <v>4</v>
       </c>
@@ -28113,7 +28157,7 @@
       <c r="F3" s="15"/>
       <c r="G3" s="16"/>
       <c r="H3" s="15"/>
-      <c r="I3" s="88"/>
+      <c r="I3" s="87"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
@@ -28134,17 +28178,17 @@
       <c r="F4" s="15"/>
       <c r="G4" s="16"/>
       <c r="H4" s="15"/>
-      <c r="I4" s="81"/>
+      <c r="I4" s="82"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="80">
+      <c r="A5" s="81">
         <v>62</v>
       </c>
-      <c r="B5" s="87" t="str">
+      <c r="B5" s="88" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/dynamic-programming/leetcode-62-unique-paths/","Unique Paths")</f>
         <v>Unique Paths</v>
       </c>
-      <c r="C5" s="83" t="s">
+      <c r="C5" s="84" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="13" t="str">
@@ -28172,9 +28216,9 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="81"/>
-      <c r="B6" s="81"/>
-      <c r="C6" s="81"/>
+      <c r="A6" s="82"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="82"/>
       <c r="D6" s="14" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/searching/leetcode-1210-minimum-moves-to-reach-target-with-rotations/","1210")</f>
         <v>1210</v>
@@ -28183,7 +28227,7 @@
       <c r="F6" s="16"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
-      <c r="I6" s="88"/>
+      <c r="I6" s="87"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
@@ -28210,7 +28254,7 @@
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
-      <c r="I7" s="81"/>
+      <c r="I7" s="82"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
@@ -28315,7 +28359,7 @@
       <c r="F11" s="15"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
-      <c r="I11" s="88"/>
+      <c r="I11" s="87"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
@@ -28333,7 +28377,7 @@
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
-      <c r="I12" s="81"/>
+      <c r="I12" s="82"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
@@ -28379,14 +28423,14 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="80">
+      <c r="A15" s="81">
         <v>72</v>
       </c>
-      <c r="B15" s="85" t="str">
+      <c r="B15" s="89" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/dynamic-programming/leetcode-72-edit-distance/","Edit Distance")</f>
         <v>Edit Distance</v>
       </c>
-      <c r="C15" s="83" t="s">
+      <c r="C15" s="84" t="s">
         <v>7</v>
       </c>
       <c r="D15" s="14" t="str">
@@ -28414,9 +28458,9 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="81"/>
-      <c r="B16" s="81"/>
-      <c r="C16" s="81"/>
+      <c r="A16" s="82"/>
+      <c r="B16" s="82"/>
+      <c r="C16" s="82"/>
       <c r="D16" s="13" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/dynamic-programming/leetcode-712-minimum-ascii-delete-sum-for-two-strings/","712")</f>
         <v>712</v>
@@ -28437,7 +28481,7 @@
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/dynamic-programming/leetcode-718-maximum-length-of-repeated-subarray/","718")</f>
         <v>718</v>
       </c>
-      <c r="I16" s="81"/>
+      <c r="I16" s="82"/>
     </row>
     <row r="17" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
@@ -28486,14 +28530,14 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A19" s="80">
+      <c r="A19" s="81">
         <v>322</v>
       </c>
-      <c r="B19" s="87" t="str">
+      <c r="B19" s="88" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/dynamic-programming/leetcode-322-coin-change/","Coin Change")</f>
         <v>Coin Change</v>
       </c>
-      <c r="C19" s="83" t="s">
+      <c r="C19" s="84" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="10" t="str">
@@ -28521,9 +28565,9 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A20" s="81"/>
-      <c r="B20" s="81"/>
-      <c r="C20" s="81"/>
+      <c r="A20" s="82"/>
+      <c r="B20" s="82"/>
+      <c r="C20" s="82"/>
       <c r="D20" s="10" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/dynamic-programming/leetcode-1220-count-vowels-permutation/","1220")</f>
         <v>1220</v>
@@ -28541,7 +28585,7 @@
         <v>1269</v>
       </c>
       <c r="H20" s="15"/>
-      <c r="I20" s="81"/>
+      <c r="I20" s="82"/>
     </row>
     <row r="21" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
@@ -34619,13 +34663,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="I5:I7"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C15:C16"/>
@@ -34634,6 +34671,13 @@
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="I19:I20"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="I5:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -34669,15 +34713,15 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="D1" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="80"/>
       <c r="K1" s="5" t="s">
         <v>4</v>
       </c>
@@ -38908,15 +38952,15 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="D1" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="80"/>
       <c r="K1" s="5" t="s">
         <v>4</v>
       </c>
@@ -43198,13 +43242,13 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="D1" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="80"/>
       <c r="I1" s="5" t="s">
         <v>4</v>
       </c>
@@ -48356,13 +48400,13 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="D1" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="80"/>
       <c r="I1" s="33" t="s">
         <v>4</v>
       </c>
@@ -53768,15 +53812,15 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="D1" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="80"/>
       <c r="K1" s="5" t="s">
         <v>4</v>
       </c>
@@ -57975,18 +58019,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="90" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="90"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
       <c r="K1" s="53"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -58036,15 +58080,15 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="77" t="s">
+      <c r="D4" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="80"/>
       <c r="K4" s="5" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Update problem 100, 1302, 590, 987
</commit_message>
<xml_diff>
--- a/Python_LeetCode/花花酱 LeetCode 题目分类 _ youtube.com_user_xxfflower .xlsx
+++ b/Python_LeetCode/花花酱 LeetCode 题目分类 _ youtube.com_user_xxfflower .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ba6ca2776cfd04a2/Projects/DevOps/Notes/DevOps-learning-notes/Python_LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="355" documentId="11_06CFFED9B2426DA59DEC10EDCE3DB48FCB33D6CA" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F0A8333A-4012-4BE6-8317-BC9FE4990F7A}"/>
+  <xr:revisionPtr revIDLastSave="377" documentId="11_06CFFED9B2426DA59DEC10EDCE3DB48FCB33D6CA" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D39A9684-9380-4B18-932E-248CC66B68CB}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="884" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -274,7 +274,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="103">
   <si>
     <t>Id</t>
   </si>
@@ -576,6 +576,18 @@
   </si>
   <si>
     <t>left = 0, right = len(nums) - 1, while left &lt; right, mid = left + (right - left) // 2,  return left if target == nums[left] else -1</t>
+  </si>
+  <si>
+    <t>590. N-ary Tree Postorder Traversal</t>
+  </si>
+  <si>
+    <t>987.Vertical Order Traversal of a Binary Tree</t>
+  </si>
+  <si>
+    <t>1302. Deepest Leaves Sum</t>
+  </si>
+  <si>
+    <t>100.Same Tree</t>
   </si>
 </sst>
 </file>
@@ -1527,11 +1539,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB87F8D1-CF69-4679-BA35-9F173745AC62}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1683,7 +1695,9 @@
       <c r="E8" s="64" t="s">
         <v>86</v>
       </c>
-      <c r="F8" s="89"/>
+      <c r="F8" s="64" t="s">
+        <v>86</v>
+      </c>
       <c r="G8" s="89"/>
     </row>
     <row r="9" spans="1:8" s="60" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -1781,6 +1795,9 @@
       <c r="C15" s="64" t="s">
         <v>86</v>
       </c>
+      <c r="D15" s="64" t="s">
+        <v>86</v>
+      </c>
       <c r="H15" t="s">
         <v>98</v>
       </c>
@@ -1829,6 +1846,9 @@
       <c r="B21" s="64" t="s">
         <v>86</v>
       </c>
+      <c r="C21" s="64" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="22" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="82">
@@ -1864,6 +1884,9 @@
       <c r="A28" s="83" t="s">
         <v>95</v>
       </c>
+      <c r="B28" s="64" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="29" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="84" t="s">
@@ -1880,6 +1903,43 @@
         <v>97</v>
       </c>
       <c r="B31" s="64" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="82">
+        <v>43952</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="83" t="s">
+        <v>99</v>
+      </c>
+      <c r="B33" s="64" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="83" t="s">
+        <v>100</v>
+      </c>
+      <c r="B34" s="64" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="83" t="s">
+        <v>101</v>
+      </c>
+      <c r="B35" s="64" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="83" t="s">
+        <v>102</v>
+      </c>
+      <c r="B36" s="64" t="s">
         <v>86</v>
       </c>
     </row>
@@ -10378,8 +10438,8 @@
   </sheetPr>
   <dimension ref="A1:L998"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14576,7 +14636,7 @@
   </sheetPr>
   <dimension ref="A1:J996"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -18707,7 +18767,7 @@
   <dimension ref="A1:K996"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -22868,7 +22928,7 @@
   <dimension ref="A1:J1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -28202,7 +28262,7 @@
   <dimension ref="A1:L999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -32469,7 +32529,7 @@
   <dimension ref="A1:L1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -41970,7 +42030,7 @@
   <dimension ref="A1:J1013"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="A15:J16"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -48652,7 +48712,7 @@
   <dimension ref="A1:J1007"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -54115,7 +54175,7 @@
   <dimension ref="A1:L1005"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update more solutions to question 146, 55, 560, 64
</commit_message>
<xml_diff>
--- a/Python_LeetCode/花花酱 LeetCode 题目分类 _ youtube.com_user_xxfflower .xlsx
+++ b/Python_LeetCode/花花酱 LeetCode 题目分类 _ youtube.com_user_xxfflower .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ba6ca2776cfd04a2/Projects/DevOps/Notes/DevOps-learning-notes/Python_LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="377" documentId="11_06CFFED9B2426DA59DEC10EDCE3DB48FCB33D6CA" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D39A9684-9380-4B18-932E-248CC66B68CB}"/>
+  <xr:revisionPtr revIDLastSave="401" documentId="11_06CFFED9B2426DA59DEC10EDCE3DB48FCB33D6CA" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9285E3CF-E5AB-4E7D-9422-B69361A96F8F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="884" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -274,7 +274,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="103">
   <si>
     <t>Id</t>
   </si>
@@ -1163,41 +1163,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="36" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1222,6 +1187,41 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1542,52 +1542,52 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.109375" style="84" customWidth="1"/>
-    <col min="2" max="4" width="2.77734375" style="90" customWidth="1"/>
-    <col min="5" max="7" width="2.77734375" style="89" customWidth="1"/>
+    <col min="1" max="1" width="27.109375" style="69" customWidth="1"/>
+    <col min="2" max="4" width="2.77734375" style="75" customWidth="1"/>
+    <col min="5" max="7" width="2.77734375" style="74" customWidth="1"/>
     <col min="8" max="8" width="96.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="63" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="81"/>
-      <c r="B1" s="85">
+      <c r="A1" s="66"/>
+      <c r="B1" s="70">
         <v>1</v>
       </c>
-      <c r="C1" s="85">
+      <c r="C1" s="70">
         <v>2</v>
       </c>
-      <c r="D1" s="85">
+      <c r="D1" s="70">
         <v>3</v>
       </c>
-      <c r="E1" s="86">
+      <c r="E1" s="71">
         <v>4</v>
       </c>
-      <c r="F1" s="87">
+      <c r="F1" s="72">
         <v>5</v>
       </c>
-      <c r="G1" s="87">
+      <c r="G1" s="72">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="62" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="82">
+      <c r="A2" s="67">
         <v>43937</v>
       </c>
       <c r="B2" s="64"/>
       <c r="C2" s="64"/>
       <c r="D2" s="64"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
     </row>
     <row r="3" spans="1:8" s="60" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="68" t="s">
         <v>78</v>
       </c>
       <c r="B3" s="64" t="s">
@@ -1605,10 +1605,10 @@
       <c r="F3" s="64" t="s">
         <v>86</v>
       </c>
-      <c r="G3" s="89"/>
+      <c r="G3" s="74"/>
     </row>
     <row r="4" spans="1:8" s="60" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="84" t="s">
+      <c r="A4" s="69" t="s">
         <v>79</v>
       </c>
       <c r="B4" s="64" t="s">
@@ -1623,22 +1623,24 @@
       <c r="E4" s="64" t="s">
         <v>86</v>
       </c>
-      <c r="F4" s="89"/>
-      <c r="G4" s="89"/>
+      <c r="F4" s="64" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" s="74"/>
     </row>
     <row r="5" spans="1:8" s="62" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="82">
+      <c r="A5" s="67">
         <v>43938</v>
       </c>
       <c r="B5" s="64"/>
       <c r="C5" s="64"/>
       <c r="D5" s="64"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="88"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
     </row>
     <row r="6" spans="1:8" s="60" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="83" t="s">
+      <c r="A6" s="68" t="s">
         <v>81</v>
       </c>
       <c r="B6" s="64" t="s">
@@ -1656,10 +1658,10 @@
       <c r="F6" s="64" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="89"/>
+      <c r="G6" s="74"/>
     </row>
     <row r="7" spans="1:8" s="60" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="83" t="s">
+      <c r="A7" s="68" t="s">
         <v>82</v>
       </c>
       <c r="B7" s="64" t="s">
@@ -1677,10 +1679,10 @@
       <c r="F7" s="64" t="s">
         <v>86</v>
       </c>
-      <c r="G7" s="89"/>
+      <c r="G7" s="74"/>
     </row>
     <row r="8" spans="1:8" s="60" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="83" t="s">
+      <c r="A8" s="68" t="s">
         <v>83</v>
       </c>
       <c r="B8" s="64" t="s">
@@ -1698,10 +1700,10 @@
       <c r="F8" s="64" t="s">
         <v>86</v>
       </c>
-      <c r="G8" s="89"/>
+      <c r="G8" s="74"/>
     </row>
     <row r="9" spans="1:8" s="60" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="83" t="s">
+      <c r="A9" s="68" t="s">
         <v>84</v>
       </c>
       <c r="B9" s="64" t="s">
@@ -1716,11 +1718,13 @@
       <c r="E9" s="64" t="s">
         <v>86</v>
       </c>
-      <c r="F9" s="89"/>
-      <c r="G9" s="89"/>
+      <c r="F9" s="64" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" s="74"/>
     </row>
     <row r="10" spans="1:8" s="60" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="83" t="s">
+      <c r="A10" s="68" t="s">
         <v>80</v>
       </c>
       <c r="B10" s="64" t="s">
@@ -1735,22 +1739,24 @@
       <c r="E10" s="64" t="s">
         <v>86</v>
       </c>
-      <c r="F10" s="89"/>
-      <c r="G10" s="89"/>
+      <c r="F10" s="64" t="s">
+        <v>86</v>
+      </c>
+      <c r="G10" s="74"/>
     </row>
     <row r="11" spans="1:8" s="62" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="82">
+      <c r="A11" s="67">
         <v>43939</v>
       </c>
       <c r="B11" s="64"/>
       <c r="C11" s="64"/>
       <c r="D11" s="64"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="88"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="73"/>
+      <c r="G11" s="73"/>
     </row>
     <row r="12" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="83" t="s">
+      <c r="A12" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B12" s="64" t="s">
@@ -1762,17 +1768,15 @@
       <c r="D12" s="64" t="s">
         <v>86</v>
       </c>
-      <c r="E12" s="64" t="s">
-        <v>86</v>
-      </c>
+      <c r="E12" s="64"/>
     </row>
     <row r="13" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="82">
+      <c r="A13" s="67">
         <v>43941</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="84" t="s">
+      <c r="A14" s="69" t="s">
         <v>87</v>
       </c>
       <c r="B14" s="64" t="s">
@@ -1784,9 +1788,12 @@
       <c r="D14" s="64" t="s">
         <v>86</v>
       </c>
+      <c r="E14" s="64" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="83" t="s">
+      <c r="A15" s="68" t="s">
         <v>88</v>
       </c>
       <c r="B15" s="64" t="s">
@@ -1798,17 +1805,20 @@
       <c r="D15" s="64" t="s">
         <v>86</v>
       </c>
+      <c r="E15" s="64" t="s">
+        <v>86</v>
+      </c>
       <c r="H15" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="82">
+      <c r="A16" s="67">
         <v>43942</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="83" t="s">
+    <row r="17" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="68" t="s">
         <v>89</v>
       </c>
       <c r="B17" s="64" t="s">
@@ -1817,14 +1827,17 @@
       <c r="C17" s="64" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="82">
+      <c r="D17" s="64" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="67">
         <v>43943</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="84" t="s">
+    <row r="19" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="69" t="s">
         <v>90</v>
       </c>
       <c r="B19" s="64" t="s">
@@ -1833,14 +1846,17 @@
       <c r="C19" s="64" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="82">
+      <c r="D19" s="64" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="67">
         <v>43945</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="83" t="s">
+    <row r="21" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="68" t="s">
         <v>91</v>
       </c>
       <c r="B21" s="64" t="s">
@@ -1849,97 +1865,133 @@
       <c r="C21" s="64" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="82">
+      <c r="D21" s="64" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="67">
         <v>43947</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="84" t="s">
+    <row r="23" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="69" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="84" t="s">
+      <c r="B23" s="64" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="69" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="82">
+      <c r="B24" s="64" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="64" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="67">
         <v>43949</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="84" t="s">
+    <row r="26" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="69" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="82">
+      <c r="B26" s="64" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" s="64" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="67">
         <v>43950</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="83" t="s">
+    <row r="28" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="68" t="s">
         <v>95</v>
       </c>
       <c r="B28" s="64" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="84" t="s">
+      <c r="C28" s="64" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="69" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="82">
+    <row r="30" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="67">
         <v>43951</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="83" t="s">
+    <row r="31" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="68" t="s">
         <v>97</v>
       </c>
       <c r="B31" s="64" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="82">
+      <c r="C31" s="64" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="67">
         <v>43952</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="83" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="68" t="s">
         <v>99</v>
       </c>
       <c r="B33" s="64" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="83" t="s">
+      <c r="C33" s="64" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="68" t="s">
         <v>100</v>
       </c>
       <c r="B34" s="64" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="83" t="s">
+      <c r="C34" s="64" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="68" t="s">
         <v>101</v>
       </c>
       <c r="B35" s="64" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="83" t="s">
+      <c r="C35" s="64" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="68" t="s">
         <v>102</v>
       </c>
       <c r="B36" s="64" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" s="64" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2022,15 +2074,15 @@
       <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="66" t="s">
+      <c r="D3" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="68"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="78"/>
       <c r="K3" s="5" t="s">
         <v>4</v>
       </c>
@@ -6269,15 +6321,15 @@
       <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="80" t="s">
+      <c r="D1" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
       <c r="K1" s="53" t="s">
         <v>4</v>
       </c>
@@ -10461,15 +10513,15 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="68"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="78"/>
       <c r="K1" s="5" t="s">
         <v>4</v>
       </c>
@@ -14659,13 +14711,13 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="68"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="78"/>
       <c r="I1" s="5" t="s">
         <v>4</v>
       </c>
@@ -18789,14 +18841,14 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="68"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="78"/>
       <c r="J1" s="5" t="s">
         <v>4</v>
       </c>
@@ -22950,26 +23002,26 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="68"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="78"/>
       <c r="I1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="69">
+      <c r="A2" s="79">
         <v>94</v>
       </c>
-      <c r="B2" s="71" t="str">
+      <c r="B2" s="81" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/tree/leetcode-94-binary-tree-inorder-traversal/","Binary Tree Inorder Traversal")</f>
         <v>Binary Tree Inorder Traversal</v>
       </c>
-      <c r="C2" s="72" t="s">
+      <c r="C2" s="82" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="10" t="str">
@@ -23000,9 +23052,9 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="70"/>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
+      <c r="A3" s="80"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
       <c r="D3" s="10" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/tree/leetcode-987-vertical-order-traversal-of-a-binary-tree/","987")</f>
         <v>987</v>
@@ -23017,14 +23069,14 @@
       <c r="I3" s="18"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="69">
+      <c r="A4" s="79">
         <v>100</v>
       </c>
-      <c r="B4" s="73" t="str">
+      <c r="B4" s="83" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/tree/leetcode-100-same-tree/","Same Tree")</f>
         <v>Same Tree</v>
       </c>
-      <c r="C4" s="72" t="s">
+      <c r="C4" s="82" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="9" t="str">
@@ -23053,9 +23105,9 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="70"/>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
+      <c r="A5" s="80"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
       <c r="D5" s="29" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/univalued-binary-tree/","965")</f>
         <v>965</v>
@@ -28284,15 +28336,15 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="68"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="78"/>
       <c r="K1" s="5" t="s">
         <v>4</v>
       </c>
@@ -32551,15 +32603,15 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="68"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="78"/>
       <c r="K1" s="5" t="s">
         <v>4</v>
       </c>
@@ -36869,13 +36921,13 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="68"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="78"/>
       <c r="I1" s="5" t="s">
         <v>4</v>
       </c>
@@ -42052,13 +42104,13 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="68"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="78"/>
       <c r="I1" s="6" t="s">
         <v>4</v>
       </c>
@@ -42085,7 +42137,7 @@
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
-      <c r="I2" s="74" t="s">
+      <c r="I2" s="85" t="s">
         <v>8</v>
       </c>
       <c r="J2">
@@ -42111,7 +42163,7 @@
       <c r="F3" s="15"/>
       <c r="G3" s="16"/>
       <c r="H3" s="15"/>
-      <c r="I3" s="75"/>
+      <c r="I3" s="87"/>
       <c r="J3">
         <v>2</v>
       </c>
@@ -42135,20 +42187,20 @@
       <c r="F4" s="15"/>
       <c r="G4" s="16"/>
       <c r="H4" s="15"/>
-      <c r="I4" s="70"/>
+      <c r="I4" s="80"/>
       <c r="J4">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="69">
+      <c r="A5" s="79">
         <v>62</v>
       </c>
-      <c r="B5" s="76" t="str">
+      <c r="B5" s="86" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/dynamic-programming/leetcode-62-unique-paths/","Unique Paths")</f>
         <v>Unique Paths</v>
       </c>
-      <c r="C5" s="72" t="s">
+      <c r="C5" s="82" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="13" t="str">
@@ -42171,7 +42223,7 @@
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/dynamic-programming/leetcode-931-minimum-falling-path-sum/","931")</f>
         <v>931</v>
       </c>
-      <c r="I5" s="74" t="s">
+      <c r="I5" s="85" t="s">
         <v>14</v>
       </c>
       <c r="J5">
@@ -42179,9 +42231,9 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="70"/>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
+      <c r="A6" s="80"/>
+      <c r="B6" s="80"/>
+      <c r="C6" s="80"/>
       <c r="D6" s="14" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/searching/leetcode-1210-minimum-moves-to-reach-target-with-rotations/","1210")</f>
         <v>1210</v>
@@ -42190,7 +42242,7 @@
       <c r="F6" s="16"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
-      <c r="I6" s="75"/>
+      <c r="I6" s="87"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
@@ -42217,7 +42269,7 @@
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
-      <c r="I7" s="70"/>
+      <c r="I7" s="80"/>
       <c r="J7">
         <v>4</v>
       </c>
@@ -42305,7 +42357,7 @@
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
-      <c r="I10" s="74" t="s">
+      <c r="I10" s="85" t="s">
         <v>20</v>
       </c>
       <c r="J10">
@@ -42334,7 +42386,7 @@
       <c r="F11" s="15"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
-      <c r="I11" s="75"/>
+      <c r="I11" s="87"/>
       <c r="J11">
         <v>3</v>
       </c>
@@ -42355,7 +42407,7 @@
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
-      <c r="I12" s="70"/>
+      <c r="I12" s="80"/>
       <c r="J12">
         <v>1</v>
       </c>
@@ -42410,14 +42462,14 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="69">
+      <c r="A15" s="79">
         <v>72</v>
       </c>
-      <c r="B15" s="77" t="str">
+      <c r="B15" s="84" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/dynamic-programming/leetcode-72-edit-distance/","Edit Distance")</f>
         <v>Edit Distance</v>
       </c>
-      <c r="C15" s="72" t="s">
+      <c r="C15" s="82" t="s">
         <v>7</v>
       </c>
       <c r="D15" s="14" t="str">
@@ -42440,7 +42492,7 @@
         <f>HYPERLINK("https://leetcode.com/problems/delete-operation-for-two-strings/","583")</f>
         <v>583</v>
       </c>
-      <c r="I15" s="74" t="s">
+      <c r="I15" s="85" t="s">
         <v>25</v>
       </c>
       <c r="J15">
@@ -42448,9 +42500,9 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="70"/>
-      <c r="B16" s="70"/>
-      <c r="C16" s="70"/>
+      <c r="A16" s="80"/>
+      <c r="B16" s="80"/>
+      <c r="C16" s="80"/>
       <c r="D16" s="13" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/dynamic-programming/leetcode-712-minimum-ascii-delete-sum-for-two-strings/","712")</f>
         <v>712</v>
@@ -42471,7 +42523,7 @@
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/dynamic-programming/leetcode-718-maximum-length-of-repeated-subarray/","718")</f>
         <v>718</v>
       </c>
-      <c r="I16" s="70"/>
+      <c r="I16" s="80"/>
     </row>
     <row r="17" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
@@ -42526,14 +42578,14 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A19" s="69">
+      <c r="A19" s="79">
         <v>322</v>
       </c>
-      <c r="B19" s="76" t="str">
+      <c r="B19" s="86" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/dynamic-programming/leetcode-322-coin-change/","Coin Change")</f>
         <v>Coin Change</v>
       </c>
-      <c r="C19" s="72" t="s">
+      <c r="C19" s="82" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="10" t="str">
@@ -42556,7 +42608,7 @@
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/leetcode/leetcode-weekly-contest-137/","1049")</f>
         <v>1049</v>
       </c>
-      <c r="I19" s="74" t="s">
+      <c r="I19" s="85" t="s">
         <v>28</v>
       </c>
       <c r="J19">
@@ -42564,9 +42616,9 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A20" s="70"/>
-      <c r="B20" s="70"/>
-      <c r="C20" s="70"/>
+      <c r="A20" s="80"/>
+      <c r="B20" s="80"/>
+      <c r="C20" s="80"/>
       <c r="D20" s="10" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/dynamic-programming/leetcode-1220-count-vowels-permutation/","1220")</f>
         <v>1220</v>
@@ -42584,7 +42636,7 @@
         <v>1269</v>
       </c>
       <c r="H20" s="15"/>
-      <c r="I20" s="70"/>
+      <c r="I20" s="80"/>
     </row>
     <row r="21" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
@@ -48684,6 +48736,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="I5:I7"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C15:C16"/>
@@ -48692,13 +48751,6 @@
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="I19:I20"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="I5:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -48734,13 +48786,13 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="68"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="78"/>
       <c r="I1" s="33" t="s">
         <v>4</v>
       </c>
@@ -54188,18 +54240,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="88" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
       <c r="K1" s="53"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -54249,15 +54301,15 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="66" t="s">
+      <c r="D4" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="68"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="78"/>
       <c r="K4" s="5" t="s">
         <v>4</v>
       </c>
@@ -58453,15 +58505,15 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="68"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="78"/>
       <c r="K1" s="5" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
update problem 1, 101, 104, 110
</commit_message>
<xml_diff>
--- a/Python_LeetCode/花花酱 LeetCode 题目分类 _ youtube.com_user_xxfflower .xlsx
+++ b/Python_LeetCode/花花酱 LeetCode 题目分类 _ youtube.com_user_xxfflower .xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ba6ca2776cfd04a2/Projects/DevOps/Notes/DevOps-learning-notes/Python_LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="401" documentId="11_06CFFED9B2426DA59DEC10EDCE3DB48FCB33D6CA" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9285E3CF-E5AB-4E7D-9422-B69361A96F8F}"/>
+  <xr:revisionPtr revIDLastSave="414" documentId="11_06CFFED9B2426DA59DEC10EDCE3DB48FCB33D6CA" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{52C97BE8-39F1-41F3-B138-8BA13E7D83A9}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="884" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -274,7 +274,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="107">
   <si>
     <t>Id</t>
   </si>
@@ -588,6 +588,18 @@
   </si>
   <si>
     <t>100.Same Tree</t>
+  </si>
+  <si>
+    <t>1.Two Sum</t>
+  </si>
+  <si>
+    <t>104. Maximum Depth of Binary Tree</t>
+  </si>
+  <si>
+    <t>101. Symmetric Tree</t>
+  </si>
+  <si>
+    <t>110. Balanced Binary Tree</t>
   </si>
 </sst>
 </file>
@@ -1004,7 +1016,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1189,6 +1201,7 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1207,16 +1220,16 @@
     <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1539,11 +1552,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB87F8D1-CF69-4679-BA35-9F173745AC62}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1817,7 +1830,7 @@
         <v>43942</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="68" t="s">
         <v>89</v>
       </c>
@@ -1831,12 +1844,12 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="67">
         <v>43943</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="69" t="s">
         <v>90</v>
       </c>
@@ -1850,12 +1863,12 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="67">
         <v>43945</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="68" t="s">
         <v>91</v>
       </c>
@@ -1868,21 +1881,27 @@
       <c r="D21" s="64" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="64" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="67">
         <v>43947</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="69" t="s">
         <v>92</v>
       </c>
       <c r="B23" s="64" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="64" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="69" t="s">
         <v>93</v>
       </c>
@@ -1892,13 +1911,16 @@
       <c r="C24" s="64" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="64" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="67">
         <v>43949</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="69" t="s">
         <v>94</v>
       </c>
@@ -1908,13 +1930,16 @@
       <c r="C26" s="64" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D26" s="64" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="67">
         <v>43950</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="68" t="s">
         <v>95</v>
       </c>
@@ -1924,18 +1949,21 @@
       <c r="C28" s="64" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D28" s="64" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="69" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="67">
         <v>43951</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="68" t="s">
         <v>97</v>
       </c>
@@ -1946,12 +1974,12 @@
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="67">
         <v>43952</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="68" t="s">
         <v>99</v>
       </c>
@@ -1962,7 +1990,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="68" t="s">
         <v>100</v>
       </c>
@@ -1973,7 +2001,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="68" t="s">
         <v>101</v>
       </c>
@@ -1984,7 +2012,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="68" t="s">
         <v>102</v>
       </c>
@@ -1993,6 +2021,40 @@
       </c>
       <c r="C36" s="64" t="s">
         <v>86</v>
+      </c>
+      <c r="D36" s="64" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="67">
+        <v>43955</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="69" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" s="76" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="69" t="s">
+        <v>105</v>
+      </c>
+      <c r="B39" s="75"/>
+      <c r="C39" s="75"/>
+      <c r="D39" s="75"/>
+      <c r="E39" s="74"/>
+      <c r="F39" s="74"/>
+      <c r="G39" s="74"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="69" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="69" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2009,7 +2071,7 @@
   <dimension ref="A1:O1004"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2074,15 +2136,15 @@
       <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="76" t="s">
+      <c r="D3" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="79"/>
       <c r="K3" s="5" t="s">
         <v>4</v>
       </c>
@@ -6321,15 +6383,15 @@
       <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="90" t="s">
+      <c r="D1" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
       <c r="K1" s="53" t="s">
         <v>4</v>
       </c>
@@ -10491,7 +10553,7 @@
   <dimension ref="A1:L998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10513,15 +10575,15 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="79"/>
       <c r="K1" s="5" t="s">
         <v>4</v>
       </c>
@@ -14711,13 +14773,13 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="79"/>
       <c r="I1" s="5" t="s">
         <v>4</v>
       </c>
@@ -18841,14 +18903,14 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="79"/>
       <c r="J1" s="5" t="s">
         <v>4</v>
       </c>
@@ -22980,7 +23042,7 @@
   <dimension ref="A1:J1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -23002,26 +23064,26 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="79"/>
       <c r="I1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="79">
+      <c r="A2" s="80">
         <v>94</v>
       </c>
-      <c r="B2" s="81" t="str">
+      <c r="B2" s="82" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/tree/leetcode-94-binary-tree-inorder-traversal/","Binary Tree Inorder Traversal")</f>
         <v>Binary Tree Inorder Traversal</v>
       </c>
-      <c r="C2" s="82" t="s">
+      <c r="C2" s="83" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="10" t="str">
@@ -23052,9 +23114,9 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="80"/>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
+      <c r="A3" s="81"/>
+      <c r="B3" s="81"/>
+      <c r="C3" s="81"/>
       <c r="D3" s="10" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/tree/leetcode-987-vertical-order-traversal-of-a-binary-tree/","987")</f>
         <v>987</v>
@@ -23069,14 +23131,14 @@
       <c r="I3" s="18"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="79">
+      <c r="A4" s="80">
         <v>100</v>
       </c>
-      <c r="B4" s="83" t="str">
+      <c r="B4" s="84" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/tree/leetcode-100-same-tree/","Same Tree")</f>
         <v>Same Tree</v>
       </c>
-      <c r="C4" s="82" t="s">
+      <c r="C4" s="83" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="9" t="str">
@@ -23105,9 +23167,9 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="80"/>
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
+      <c r="A5" s="81"/>
+      <c r="B5" s="81"/>
+      <c r="C5" s="81"/>
       <c r="D5" s="29" t="str">
         <f>HYPERLINK("https://leetcode.com/problems/univalued-binary-tree/","965")</f>
         <v>965</v>
@@ -28336,15 +28398,15 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="79"/>
       <c r="K1" s="5" t="s">
         <v>4</v>
       </c>
@@ -32603,15 +32665,15 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="79"/>
       <c r="K1" s="5" t="s">
         <v>4</v>
       </c>
@@ -36921,13 +36983,13 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="79"/>
       <c r="I1" s="5" t="s">
         <v>4</v>
       </c>
@@ -42104,13 +42166,13 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="79"/>
       <c r="I1" s="6" t="s">
         <v>4</v>
       </c>
@@ -42163,7 +42225,7 @@
       <c r="F3" s="15"/>
       <c r="G3" s="16"/>
       <c r="H3" s="15"/>
-      <c r="I3" s="87"/>
+      <c r="I3" s="86"/>
       <c r="J3">
         <v>2</v>
       </c>
@@ -42187,20 +42249,20 @@
       <c r="F4" s="15"/>
       <c r="G4" s="16"/>
       <c r="H4" s="15"/>
-      <c r="I4" s="80"/>
+      <c r="I4" s="81"/>
       <c r="J4">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="79">
+      <c r="A5" s="80">
         <v>62</v>
       </c>
-      <c r="B5" s="86" t="str">
+      <c r="B5" s="87" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/dynamic-programming/leetcode-62-unique-paths/","Unique Paths")</f>
         <v>Unique Paths</v>
       </c>
-      <c r="C5" s="82" t="s">
+      <c r="C5" s="83" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="13" t="str">
@@ -42231,9 +42293,9 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="80"/>
-      <c r="B6" s="80"/>
-      <c r="C6" s="80"/>
+      <c r="A6" s="81"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="81"/>
       <c r="D6" s="14" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/searching/leetcode-1210-minimum-moves-to-reach-target-with-rotations/","1210")</f>
         <v>1210</v>
@@ -42242,7 +42304,7 @@
       <c r="F6" s="16"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
-      <c r="I6" s="87"/>
+      <c r="I6" s="86"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
@@ -42269,7 +42331,7 @@
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
-      <c r="I7" s="80"/>
+      <c r="I7" s="81"/>
       <c r="J7">
         <v>4</v>
       </c>
@@ -42386,7 +42448,7 @@
       <c r="F11" s="15"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
-      <c r="I11" s="87"/>
+      <c r="I11" s="86"/>
       <c r="J11">
         <v>3</v>
       </c>
@@ -42407,7 +42469,7 @@
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
-      <c r="I12" s="80"/>
+      <c r="I12" s="81"/>
       <c r="J12">
         <v>1</v>
       </c>
@@ -42462,14 +42524,14 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="79">
+      <c r="A15" s="80">
         <v>72</v>
       </c>
-      <c r="B15" s="84" t="str">
+      <c r="B15" s="88" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/dynamic-programming/leetcode-72-edit-distance/","Edit Distance")</f>
         <v>Edit Distance</v>
       </c>
-      <c r="C15" s="82" t="s">
+      <c r="C15" s="83" t="s">
         <v>7</v>
       </c>
       <c r="D15" s="14" t="str">
@@ -42500,9 +42562,9 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="80"/>
-      <c r="B16" s="80"/>
-      <c r="C16" s="80"/>
+      <c r="A16" s="81"/>
+      <c r="B16" s="81"/>
+      <c r="C16" s="81"/>
       <c r="D16" s="13" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/dynamic-programming/leetcode-712-minimum-ascii-delete-sum-for-two-strings/","712")</f>
         <v>712</v>
@@ -42523,7 +42585,7 @@
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/dynamic-programming/leetcode-718-maximum-length-of-repeated-subarray/","718")</f>
         <v>718</v>
       </c>
-      <c r="I16" s="80"/>
+      <c r="I16" s="81"/>
     </row>
     <row r="17" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
@@ -42578,14 +42640,14 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A19" s="79">
+      <c r="A19" s="80">
         <v>322</v>
       </c>
-      <c r="B19" s="86" t="str">
+      <c r="B19" s="87" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/dynamic-programming/leetcode-322-coin-change/","Coin Change")</f>
         <v>Coin Change</v>
       </c>
-      <c r="C19" s="82" t="s">
+      <c r="C19" s="83" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="10" t="str">
@@ -42616,9 +42678,9 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A20" s="80"/>
-      <c r="B20" s="80"/>
-      <c r="C20" s="80"/>
+      <c r="A20" s="81"/>
+      <c r="B20" s="81"/>
+      <c r="C20" s="81"/>
       <c r="D20" s="10" t="str">
         <f>HYPERLINK("https://zxi.mytechroad.com/blog/dynamic-programming/leetcode-1220-count-vowels-permutation/","1220")</f>
         <v>1220</v>
@@ -42636,7 +42698,7 @@
         <v>1269</v>
       </c>
       <c r="H20" s="15"/>
-      <c r="I20" s="80"/>
+      <c r="I20" s="81"/>
     </row>
     <row r="21" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
@@ -48736,13 +48798,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="I5:I7"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C15:C16"/>
@@ -48751,6 +48806,13 @@
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="I19:I20"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="I5:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -48786,13 +48848,13 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="79"/>
       <c r="I1" s="33" t="s">
         <v>4</v>
       </c>
@@ -54240,18 +54302,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="89" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
       <c r="K1" s="53"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -54301,15 +54363,15 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="76" t="s">
+      <c r="D4" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="77"/>
-      <c r="J4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="78"/>
+      <c r="J4" s="79"/>
       <c r="K4" s="5" t="s">
         <v>4</v>
       </c>
@@ -58505,15 +58567,15 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="79"/>
       <c r="K1" s="5" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
update new solution to problem 987
</commit_message>
<xml_diff>
--- a/Python_LeetCode/花花酱 LeetCode 题目分类 _ youtube.com_user_xxfflower .xlsx
+++ b/Python_LeetCode/花花酱 LeetCode 题目分类 _ youtube.com_user_xxfflower .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ba6ca2776cfd04a2/Projects/DevOps/Notes/DevOps-learning-notes/Python_LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="414" documentId="11_06CFFED9B2426DA59DEC10EDCE3DB48FCB33D6CA" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{52C97BE8-39F1-41F3-B138-8BA13E7D83A9}"/>
+  <xr:revisionPtr revIDLastSave="416" documentId="11_06CFFED9B2426DA59DEC10EDCE3DB48FCB33D6CA" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6A7F943A-2051-4417-9CB8-AE150E2BB2FC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="884" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -274,7 +274,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="107">
   <si>
     <t>Id</t>
   </si>
@@ -1556,7 +1556,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
+      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1973,6 +1973,9 @@
       <c r="C31" s="64" t="s">
         <v>86</v>
       </c>
+      <c r="D31" s="64" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="67">
@@ -1987,6 +1990,9 @@
         <v>86</v>
       </c>
       <c r="C33" s="64" t="s">
+        <v>86</v>
+      </c>
+      <c r="D33" s="64" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>